<commit_message>
Fixed HKCD excel file
</commit_message>
<xml_diff>
--- a/dat/climate/changzhou_climate(clean).xlsx
+++ b/dat/climate/changzhou_climate(clean).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (NHRI Taiwan)\Workspace\Github\DengueForecastHK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tirunesh\Documents\dengue-forecast-hk\dat\climate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20022" windowHeight="8227"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20025" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -475,14 +475,14 @@
       <selection activeCell="H129" sqref="H129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="13" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -524,7 +524,7 @@
       </c>
       <c r="N1" s="10"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2002</v>
       </c>
@@ -566,7 +566,7 @@
       </c>
       <c r="N2" s="10"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2002</v>
       </c>
@@ -608,7 +608,7 @@
       </c>
       <c r="N3" s="10"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2002</v>
       </c>
@@ -649,7 +649,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2002</v>
       </c>
@@ -690,7 +690,7 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2002</v>
       </c>
@@ -731,7 +731,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2002</v>
       </c>
@@ -772,7 +772,7 @@
         <v>21.2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2002</v>
       </c>
@@ -813,7 +813,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2003</v>
       </c>
@@ -854,7 +854,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2003</v>
       </c>
@@ -895,7 +895,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2003</v>
       </c>
@@ -936,7 +936,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2003</v>
       </c>
@@ -977,7 +977,7 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2003</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>20.100000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2003</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2003</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2004</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2004</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2004</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2004</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2004</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2004</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2004</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2005</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2005</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2005</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2005</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2005</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>18.8</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2005</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2005</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2006</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2006</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2006</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2006</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2006</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>19.3</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2006</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>17.3</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2006</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>20.5</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2007</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2007</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2007</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2007</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2007</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2007</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2007</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>17.3</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2008</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2008</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2008</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2008</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2008</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2008</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2008</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2009</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2009</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2009</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2009</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2009</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2009</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2009</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2010</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2010</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2010</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2010</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2010</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2010</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2010</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2011</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2011</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>14.6</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2011</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2011</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2011</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>14.6</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2011</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2011</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2012</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2012</v>
       </c>
@@ -3478,7 +3478,7 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2012</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2012</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2012</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2012</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2012</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2013</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2013</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2013</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2013</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2013</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2013</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2013</v>
       </c>
@@ -3970,7 +3970,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2014</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>17.3</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2014</v>
       </c>
@@ -4052,7 +4052,7 @@
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2014</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2014</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2014</v>
       </c>
@@ -4175,7 +4175,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2014</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2014</v>
       </c>
@@ -4257,7 +4257,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2015</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2015</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2015</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2015</v>
       </c>
@@ -4421,7 +4421,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2015</v>
       </c>
@@ -4462,7 +4462,7 @@
         <v>17.3</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2015</v>
       </c>
@@ -4503,7 +4503,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2015</v>
       </c>
@@ -4544,7 +4544,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2016</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2016</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2016</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2016</v>
       </c>
@@ -4708,7 +4708,7 @@
         <v>14.6</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2016</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2016</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2016</v>
       </c>
@@ -4831,7 +4831,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2017</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2017</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2017</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2017</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2017</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2017</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2017</v>
       </c>
@@ -5118,7 +5118,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2018</v>
       </c>
@@ -5159,7 +5159,7 @@
         <v>20.100000000000001</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>2018</v>
       </c>
@@ -5200,7 +5200,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>2018</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2018</v>
       </c>
@@ -5282,7 +5282,7 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2018</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2018</v>
       </c>
@@ -5364,7 +5364,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>2018</v>
       </c>
@@ -5405,7 +5405,7 @@
         <v>21.1</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G121" t="s">
         <v>0</v>
       </c>

</xml_diff>